<commit_message>
create gitignore, encode model and stack
</commit_message>
<xml_diff>
--- a/OPCODE-uri.xlsx
+++ b/OPCODE-uri.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\Anul 3\Semestrul 2\Arhitectura sistemelor de calcul\Proiect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\arhitectura_microprocesor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A12E1BC-B5C2-4FFF-8D67-E7EC231F81F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757E5005-8B61-4211-BFD5-09F5C551654A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="630" windowWidth="22290" windowHeight="12960" xr2:uid="{C3266503-3D4A-4217-883A-3F21B09D5F64}"/>
+    <workbookView xWindow="435" yWindow="1140" windowWidth="22290" windowHeight="12960" activeTab="2" xr2:uid="{C3266503-3D4A-4217-883A-3F21B09D5F64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="219">
   <si>
     <t>Opcode</t>
   </si>
@@ -539,13 +540,157 @@
   </si>
   <si>
     <t>Mod de adresare</t>
+  </si>
+  <si>
+    <t>PdA, PdM , Cin, SUM, PdALU, PmA, TI1</t>
+  </si>
+  <si>
+    <t>Cout : A(1)C</t>
+  </si>
+  <si>
+    <t>Cout : A(0)C</t>
+  </si>
+  <si>
+    <t>ZR : A(1)Z</t>
+  </si>
+  <si>
+    <t>ZR : A(0)Z</t>
+  </si>
+  <si>
+    <t>SR : A(1)S</t>
+  </si>
+  <si>
+    <t>SR : A(0)S</t>
+  </si>
+  <si>
+    <t>DCRSUB : A(1)V</t>
+  </si>
+  <si>
+    <t>DCRSUB : A(0)V</t>
+  </si>
+  <si>
+    <t>INTR : TIF</t>
+  </si>
+  <si>
+    <t>INTR : TINT</t>
+  </si>
+  <si>
+    <t>Flags</t>
+  </si>
+  <si>
+    <t>Instructiune</t>
+  </si>
+  <si>
+    <t>Semnale</t>
+  </si>
+  <si>
+    <t>PdA, PdM, SUM, PdALU, PmA, TI1</t>
+  </si>
+  <si>
+    <t>PdA, PdM , Cin, SUM, PdALU, TI1</t>
+  </si>
+  <si>
+    <t>PdA, PdM, AND, PdALU, PmA, TI1</t>
+  </si>
+  <si>
+    <t>Pd0s, PdM, Cin, SUM, PdALU, TI1</t>
+  </si>
+  <si>
+    <t>AD : PmRG</t>
+  </si>
+  <si>
+    <t>AI : WR</t>
+  </si>
+  <si>
+    <t>AX : WR</t>
+  </si>
+  <si>
+    <t>V : A(1)V</t>
+  </si>
+  <si>
+    <t>V : A(0)V</t>
+  </si>
+  <si>
+    <t>S : A(0)S</t>
+  </si>
+  <si>
+    <t>S : A(1)S</t>
+  </si>
+  <si>
+    <t>Z : A(0)Z</t>
+  </si>
+  <si>
+    <t>Z : A(1)Z</t>
+  </si>
+  <si>
+    <t>C : A(0)C</t>
+  </si>
+  <si>
+    <t>C : A(1)C</t>
+  </si>
+  <si>
+    <t>Pd-1s, PdM, SUM, PdALU, TI1</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>Pd_XX, SBUS, PdALU, TI1</t>
+  </si>
+  <si>
+    <t>PmPC, TI1</t>
+  </si>
+  <si>
+    <t>AM : PdIR[OP], PdPC, SUM, PdALU</t>
+  </si>
+  <si>
+    <t>AM : PdADR</t>
+  </si>
+  <si>
+    <t>PdA, SBUS , PdALU, PmA, TI1</t>
+  </si>
+  <si>
+    <t>Impuls</t>
+  </si>
+  <si>
+    <t>I1</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>I3</t>
+  </si>
+  <si>
+    <t>-2SP</t>
+  </si>
+  <si>
+    <t>PdSP, SBUS,</t>
+  </si>
+  <si>
+    <t>PdALU, PmADR</t>
+  </si>
+  <si>
+    <t>PdA, SBUS, PdALU, WR, TI1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUSH </t>
+  </si>
+  <si>
+    <t>PdSP, SBUS, PdALU,</t>
+  </si>
+  <si>
+    <t>PmADR</t>
+  </si>
+  <si>
+    <t>RD, PdMEM, PmA, +2SP, TI1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,16 +704,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="35">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1016,11 +1175,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1057,6 +1284,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1096,17 +1332,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1424,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD33FED-E2E6-4014-BFFE-C02D74BAA994}">
   <dimension ref="A1:BB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -1468,68 +1761,68 @@
     </row>
     <row r="2" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
-      <c r="B2" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46" t="s">
+      <c r="B2" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46" t="s">
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46" t="s">
+      <c r="M2" s="33"/>
+      <c r="N2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="47"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="34"/>
       <c r="R2" s="9"/>
       <c r="S2" s="2"/>
-      <c r="T2" s="46" t="s">
+      <c r="T2" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="46"/>
-      <c r="AA2" s="46"/>
-      <c r="AB2" s="46" t="s">
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="AC2" s="46"/>
-      <c r="AD2" s="46"/>
-      <c r="AE2" s="46"/>
-      <c r="AF2" s="46"/>
-      <c r="AG2" s="46"/>
-      <c r="AH2" s="46"/>
-      <c r="AI2" s="47"/>
-      <c r="AK2" s="35" t="s">
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="34"/>
+      <c r="AK2" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="AL2" s="36"/>
-      <c r="AM2" s="37" t="s">
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="AN2" s="38"/>
-      <c r="AO2" s="38"/>
-      <c r="AP2" s="38"/>
-      <c r="AQ2" s="38"/>
-      <c r="AR2" s="38"/>
-      <c r="AS2" s="38"/>
-      <c r="AT2" s="36"/>
+      <c r="AN2" s="41"/>
+      <c r="AO2" s="41"/>
+      <c r="AP2" s="41"/>
+      <c r="AQ2" s="41"/>
+      <c r="AR2" s="41"/>
+      <c r="AS2" s="41"/>
+      <c r="AT2" s="39"/>
       <c r="BB2" s="9"/>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
@@ -1602,16 +1895,16 @@
       <c r="AL3" s="13">
         <v>0</v>
       </c>
-      <c r="AM3" s="39" t="s">
+      <c r="AM3" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="AN3" s="40"/>
-      <c r="AO3" s="40"/>
-      <c r="AP3" s="40"/>
-      <c r="AQ3" s="40"/>
-      <c r="AR3" s="40"/>
-      <c r="AS3" s="40"/>
-      <c r="AT3" s="41"/>
+      <c r="AN3" s="43"/>
+      <c r="AO3" s="43"/>
+      <c r="AP3" s="43"/>
+      <c r="AQ3" s="43"/>
+      <c r="AR3" s="43"/>
+      <c r="AS3" s="43"/>
+      <c r="AT3" s="44"/>
       <c r="BB3" s="8"/>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
@@ -1684,16 +1977,16 @@
       <c r="AL4" s="4">
         <v>1</v>
       </c>
-      <c r="AM4" s="42" t="s">
+      <c r="AM4" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="AN4" s="43"/>
-      <c r="AO4" s="43"/>
-      <c r="AP4" s="43"/>
-      <c r="AQ4" s="43"/>
-      <c r="AR4" s="43"/>
-      <c r="AS4" s="43"/>
-      <c r="AT4" s="44"/>
+      <c r="AN4" s="46"/>
+      <c r="AO4" s="46"/>
+      <c r="AP4" s="46"/>
+      <c r="AQ4" s="46"/>
+      <c r="AR4" s="46"/>
+      <c r="AS4" s="46"/>
+      <c r="AT4" s="47"/>
       <c r="BB4" s="8"/>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
@@ -1766,16 +2059,16 @@
       <c r="AL5" s="4">
         <v>0</v>
       </c>
-      <c r="AM5" s="42" t="s">
+      <c r="AM5" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="AN5" s="43"/>
-      <c r="AO5" s="43"/>
-      <c r="AP5" s="43"/>
-      <c r="AQ5" s="43"/>
-      <c r="AR5" s="43"/>
-      <c r="AS5" s="43"/>
-      <c r="AT5" s="44"/>
+      <c r="AN5" s="46"/>
+      <c r="AO5" s="46"/>
+      <c r="AP5" s="46"/>
+      <c r="AQ5" s="46"/>
+      <c r="AR5" s="46"/>
+      <c r="AS5" s="46"/>
+      <c r="AT5" s="47"/>
       <c r="BB5" s="8"/>
     </row>
     <row r="6" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1848,16 +2141,16 @@
       <c r="AL6" s="7">
         <v>1</v>
       </c>
-      <c r="AM6" s="37" t="s">
+      <c r="AM6" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="AN6" s="38"/>
-      <c r="AO6" s="38"/>
-      <c r="AP6" s="38"/>
-      <c r="AQ6" s="38"/>
-      <c r="AR6" s="38"/>
-      <c r="AS6" s="38"/>
-      <c r="AT6" s="36"/>
+      <c r="AN6" s="41"/>
+      <c r="AO6" s="41"/>
+      <c r="AP6" s="41"/>
+      <c r="AQ6" s="41"/>
+      <c r="AR6" s="41"/>
+      <c r="AS6" s="41"/>
+      <c r="AT6" s="39"/>
       <c r="BB6" s="8"/>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
@@ -2193,56 +2486,56 @@
     </row>
     <row r="14" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46" t="s">
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="M14" s="46"/>
-      <c r="N14" s="46" t="s">
+      <c r="M14" s="33"/>
+      <c r="N14" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="47"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="34"/>
       <c r="S14" s="26"/>
-      <c r="T14" s="45" t="s">
+      <c r="T14" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="U14" s="46"/>
-      <c r="V14" s="46"/>
-      <c r="W14" s="46"/>
-      <c r="X14" s="46"/>
-      <c r="Y14" s="46"/>
-      <c r="Z14" s="46"/>
-      <c r="AA14" s="46"/>
-      <c r="AB14" s="46"/>
-      <c r="AC14" s="46"/>
-      <c r="AD14" s="46"/>
-      <c r="AE14" s="46"/>
-      <c r="AF14" s="46"/>
-      <c r="AG14" s="46"/>
-      <c r="AH14" s="47"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="33"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="33"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="33"/>
+      <c r="AA14" s="33"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="33"/>
+      <c r="AD14" s="33"/>
+      <c r="AE14" s="33"/>
+      <c r="AF14" s="33"/>
+      <c r="AG14" s="33"/>
+      <c r="AH14" s="34"/>
       <c r="AJ14" s="8"/>
       <c r="AL14" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="AM14" s="32" t="s">
+      <c r="AM14" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="AN14" s="33"/>
-      <c r="AO14" s="33"/>
-      <c r="AP14" s="34"/>
+      <c r="AN14" s="36"/>
+      <c r="AO14" s="36"/>
+      <c r="AP14" s="37"/>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
@@ -4025,6 +4318,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AM14:AP14"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AM6:AT6"/>
+    <mergeCell ref="AM2:AT2"/>
+    <mergeCell ref="AM3:AT3"/>
+    <mergeCell ref="AM4:AT4"/>
+    <mergeCell ref="AM5:AT5"/>
     <mergeCell ref="B14:K14"/>
     <mergeCell ref="L14:M14"/>
     <mergeCell ref="N14:Q14"/>
@@ -4036,13 +4336,6 @@
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="AM14:AP14"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AM6:AT6"/>
-    <mergeCell ref="AM2:AT2"/>
-    <mergeCell ref="AM3:AT3"/>
-    <mergeCell ref="AM4:AT4"/>
-    <mergeCell ref="AM5:AT5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4054,7 +4347,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4120,7 +4413,7 @@
       <c r="J2" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="46"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="14" t="s">
         <v>58</v>
       </c>
@@ -4727,4 +5020,865 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17310EBE-57D2-4FB4-9248-5EA040377F05}">
+  <dimension ref="A1:K56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="49"/>
+    <col min="4" max="4" width="11.7109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="49"/>
+    <col min="7" max="7" width="11.7109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="49"/>
+    <col min="10" max="10" width="11.7109375" style="49" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.7109375" style="49" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="49"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" s="51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" s="50" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="G3" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3" s="53" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="52"/>
+      <c r="B4" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="52"/>
+      <c r="E4" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="52"/>
+      <c r="H4" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="52"/>
+      <c r="B5" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="53" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="B6" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="G6" s="52"/>
+      <c r="H6" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="J6" s="52"/>
+      <c r="K6" s="53" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="52"/>
+      <c r="B7" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="G7" s="52"/>
+      <c r="H7" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="J7" s="52"/>
+      <c r="K7" s="53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="G8" s="52"/>
+      <c r="H8" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="J8" s="52"/>
+      <c r="K8" s="53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" s="52"/>
+      <c r="H9" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="J9" s="52"/>
+      <c r="K9" s="53"/>
+    </row>
+    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="52"/>
+      <c r="E10" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="52"/>
+      <c r="H10" s="53" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" s="52"/>
+      <c r="K10" s="53"/>
+    </row>
+    <row r="11" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="52"/>
+      <c r="B11" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="G11" s="52"/>
+      <c r="H11" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="J11" s="52"/>
+      <c r="K11" s="53"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
+      <c r="B12" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="52"/>
+      <c r="E12" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="G12" s="52"/>
+      <c r="H12" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="J12" s="52"/>
+      <c r="K12" s="53"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="E14" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="H14" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="J14" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="K14" s="51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="63" t="s">
+        <v>184</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>184</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="J15" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="K15" s="50" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="64"/>
+      <c r="B16" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="D16" s="58"/>
+      <c r="E16" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="G16" s="61"/>
+      <c r="H16" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="J16" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="K16" s="55" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="64"/>
+      <c r="B17" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="58"/>
+      <c r="E17" s="55" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="61"/>
+      <c r="H17" s="53" t="s">
+        <v>190</v>
+      </c>
+      <c r="J17" s="52"/>
+      <c r="K17" s="53" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="65"/>
+      <c r="B18" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="59"/>
+      <c r="E18" s="55" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" s="62"/>
+      <c r="H18" s="53" t="s">
+        <v>191</v>
+      </c>
+      <c r="J18" s="52"/>
+      <c r="K18" s="53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="H19" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="J19" s="52"/>
+      <c r="K19" s="53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
+      <c r="B20" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="D20" s="58"/>
+      <c r="E20" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="52"/>
+      <c r="H20" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="J20" s="52"/>
+      <c r="K20" s="53"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="58"/>
+      <c r="B21" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="D21" s="58"/>
+      <c r="E21" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" s="52"/>
+      <c r="H21" s="53"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="53"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
+      <c r="B22" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" s="58"/>
+      <c r="E22" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="G22" s="52"/>
+      <c r="H22" s="53"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="53"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="58"/>
+      <c r="B23" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="D23" s="58"/>
+      <c r="E23" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="G23" s="52"/>
+      <c r="H23" s="53"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="53"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
+      <c r="B24" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="58"/>
+      <c r="E24" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="G24" s="52"/>
+      <c r="H24" s="53"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="53"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
+      <c r="B25" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="D25" s="58"/>
+      <c r="E25" s="53" t="s">
+        <v>192</v>
+      </c>
+      <c r="G25" s="52"/>
+      <c r="H25" s="53"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="58"/>
+      <c r="B26" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="D26" s="58"/>
+      <c r="E26" s="50" t="s">
+        <v>193</v>
+      </c>
+      <c r="G26" s="52"/>
+      <c r="H26" s="50"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="50"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="58"/>
+      <c r="B27" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="58"/>
+      <c r="E27" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="G27" s="52"/>
+      <c r="H27" s="50"/>
+      <c r="J27" s="52"/>
+      <c r="K27" s="50"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="59"/>
+      <c r="B28" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="D28" s="59"/>
+      <c r="E28" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="G28" s="52"/>
+      <c r="H28" s="50"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="50"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B30" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="E30" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="50"/>
+      <c r="H30" s="51"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="51"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="B31" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="57" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" s="50" t="s">
+        <v>200</v>
+      </c>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50"/>
+      <c r="J31" s="50"/>
+      <c r="K31" s="50"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="B32" s="56" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="58"/>
+      <c r="E32" s="56" t="s">
+        <v>189</v>
+      </c>
+      <c r="G32" s="52"/>
+      <c r="H32" s="56"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="56"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="52"/>
+      <c r="B33" s="56" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33" s="58"/>
+      <c r="E33" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="G33" s="52"/>
+      <c r="H33" s="53"/>
+      <c r="J33" s="52"/>
+      <c r="K33" s="53"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="52"/>
+      <c r="B34" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="D34" s="59"/>
+      <c r="E34" s="56" t="s">
+        <v>191</v>
+      </c>
+      <c r="G34" s="52"/>
+      <c r="H34" s="53"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="53"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="52"/>
+      <c r="B35" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="D35" s="57" t="s">
+        <v>182</v>
+      </c>
+      <c r="E35" s="53" t="s">
+        <v>172</v>
+      </c>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="53"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="52"/>
+      <c r="B36" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" s="58"/>
+      <c r="E36" s="53" t="s">
+        <v>173</v>
+      </c>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="53"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="52"/>
+      <c r="B37" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="D37" s="58"/>
+      <c r="E37" s="53" t="s">
+        <v>174</v>
+      </c>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="53"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="53" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" s="52"/>
+      <c r="H38" s="53"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="53"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
+      <c r="J39" s="52"/>
+      <c r="K39" s="53"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="52"/>
+      <c r="B40" s="53"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="53" t="s">
+        <v>177</v>
+      </c>
+      <c r="G40" s="52"/>
+      <c r="H40" s="53"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="53"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="52"/>
+      <c r="B41" s="53"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="53" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" s="52"/>
+      <c r="H41" s="53"/>
+      <c r="J41" s="52"/>
+      <c r="K41" s="53"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="52"/>
+      <c r="B42" s="50"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="G42" s="52"/>
+      <c r="H42" s="50"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="50"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="52"/>
+      <c r="B43" s="50"/>
+      <c r="D43" s="58"/>
+      <c r="E43" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="G43" s="52"/>
+      <c r="H43" s="50"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="50"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="52"/>
+      <c r="B44" s="50"/>
+      <c r="D44" s="59"/>
+      <c r="E44" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="G44" s="52"/>
+      <c r="H44" s="50"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="50"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B46" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="C47" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="D47" s="51" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" s="57" t="s">
+        <v>211</v>
+      </c>
+      <c r="C48" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="D48" s="67" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="52"/>
+      <c r="B49" s="58"/>
+      <c r="C49" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49" s="53" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="52"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="B52" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="66"/>
+      <c r="D52" s="70"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="51" t="s">
+        <v>208</v>
+      </c>
+      <c r="C53" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="D53" s="68"/>
+    </row>
+    <row r="54" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" s="54" t="s">
+        <v>216</v>
+      </c>
+      <c r="C54" s="67" t="s">
+        <v>218</v>
+      </c>
+      <c r="D54" s="69"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="52"/>
+      <c r="B55" s="54" t="s">
+        <v>217</v>
+      </c>
+      <c r="C55" s="53" t="s">
+        <v>180</v>
+      </c>
+      <c r="D55" s="69"/>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="52"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="53" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A32:A44"/>
+    <mergeCell ref="D35:D44"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="G19:G28"/>
+    <mergeCell ref="D15:D18"/>
+    <mergeCell ref="D19:D28"/>
+    <mergeCell ref="A19:A28"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="J16:J28"/>
+    <mergeCell ref="G32:G44"/>
+    <mergeCell ref="J32:J44"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="D3:D12"/>
+    <mergeCell ref="G3:G12"/>
+    <mergeCell ref="J3:J12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>